<commit_message>
updates to simulation study scenarios
</commit_message>
<xml_diff>
--- a/scripts/dataSims/IPM sim spreadsheet.xlsx
+++ b/scripts/dataSims/IPM sim spreadsheet.xlsx
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aebratt/Desktop/IPM_sim/scripts/dataSims/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7877DD-5B13-B841-BF26-11A7735A8CBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79164491-73D1-324F-BCE7-FB9470D468B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -83,7 +94,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -136,6 +147,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -281,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -395,6 +412,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,7 +669,7 @@
   <dimension ref="A1:AD996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:K1"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -701,15 +721,15 @@
         <v>0.3</v>
       </c>
       <c r="H2" s="6">
+        <v>0.77</v>
+      </c>
+      <c r="I2" s="6">
         <v>0.3</v>
       </c>
-      <c r="I2" s="6">
-        <v>0.2</v>
-      </c>
       <c r="J2" s="6">
-        <v>1</v>
-      </c>
-      <c r="K2" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="K2" s="7">
         <v>0.97499999999999998</v>
       </c>
     </row>
@@ -728,16 +748,16 @@
         <v>0.5</v>
       </c>
       <c r="H3" s="6">
-        <v>0.5</v>
+        <v>0.77</v>
       </c>
       <c r="I3" s="6">
         <v>0.4</v>
       </c>
       <c r="J3" s="6">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="K3" s="6">
-        <v>0.99</v>
+        <v>0.97499999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -754,17 +774,17 @@
       <c r="G4" s="7">
         <v>0.85</v>
       </c>
-      <c r="H4" s="6">
-        <v>0.8</v>
+      <c r="H4" s="43">
+        <v>0.77</v>
       </c>
       <c r="I4" s="6">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="J4" s="6">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="K4" s="6">
-        <v>0.995</v>
+        <v>0.97499999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>